<commit_message>
added pagination in publications page
</commit_message>
<xml_diff>
--- a/data/publications.xlsx
+++ b/data/publications.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\ml_lab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629543F1-66FD-4DC0-94A0-AEA3B8C7C471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C5DC30-77D7-4643-B079-A7C930A640CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1935" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{6E3728D4-265A-4CAF-8F13-4DC270A007CD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1BA501D-43AC-4B9E-AE24-5491770A7671}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="A122" sqref="A122:B133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,6 +442,1030 @@
         <v>25</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>2</v>
+      </c>
+      <c r="B50">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>2</v>
+      </c>
+      <c r="B62">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>3</v>
+      </c>
+      <c r="B63">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>4</v>
+      </c>
+      <c r="B64">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>2</v>
+      </c>
+      <c r="B66">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>3</v>
+      </c>
+      <c r="B67">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>4</v>
+      </c>
+      <c r="B68">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>5</v>
+      </c>
+      <c r="B69">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>3</v>
+      </c>
+      <c r="B71">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>4</v>
+      </c>
+      <c r="B72">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>2</v>
+      </c>
+      <c r="B74">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>3</v>
+      </c>
+      <c r="B75">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>4</v>
+      </c>
+      <c r="B76">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>2</v>
+      </c>
+      <c r="B78">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>3</v>
+      </c>
+      <c r="B79">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>4</v>
+      </c>
+      <c r="B80">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>5</v>
+      </c>
+      <c r="B81">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>2</v>
+      </c>
+      <c r="B82">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>3</v>
+      </c>
+      <c r="B83">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>4</v>
+      </c>
+      <c r="B84">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>5</v>
+      </c>
+      <c r="B85">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>2</v>
+      </c>
+      <c r="B86">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>3</v>
+      </c>
+      <c r="B87">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>4</v>
+      </c>
+      <c r="B88">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>5</v>
+      </c>
+      <c r="B89">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>2</v>
+      </c>
+      <c r="B90">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>3</v>
+      </c>
+      <c r="B91">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>4</v>
+      </c>
+      <c r="B92">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>5</v>
+      </c>
+      <c r="B93">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>2</v>
+      </c>
+      <c r="B94">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>3</v>
+      </c>
+      <c r="B95">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>4</v>
+      </c>
+      <c r="B96">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>5</v>
+      </c>
+      <c r="B97">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>2</v>
+      </c>
+      <c r="B98">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>3</v>
+      </c>
+      <c r="B99">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>4</v>
+      </c>
+      <c r="B100">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>5</v>
+      </c>
+      <c r="B101">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>2</v>
+      </c>
+      <c r="B102">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>3</v>
+      </c>
+      <c r="B103">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>4</v>
+      </c>
+      <c r="B104">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>5</v>
+      </c>
+      <c r="B105">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>2</v>
+      </c>
+      <c r="B106">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>3</v>
+      </c>
+      <c r="B107">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>4</v>
+      </c>
+      <c r="B108">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>5</v>
+      </c>
+      <c r="B109">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>2</v>
+      </c>
+      <c r="B110">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>3</v>
+      </c>
+      <c r="B111">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>4</v>
+      </c>
+      <c r="B112">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>5</v>
+      </c>
+      <c r="B113">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>2</v>
+      </c>
+      <c r="B114">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>3</v>
+      </c>
+      <c r="B115">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>4</v>
+      </c>
+      <c r="B116">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>5</v>
+      </c>
+      <c r="B117">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>2</v>
+      </c>
+      <c r="B118">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>3</v>
+      </c>
+      <c r="B119">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>4</v>
+      </c>
+      <c r="B120">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>5</v>
+      </c>
+      <c r="B121">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>2</v>
+      </c>
+      <c r="B122">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>3</v>
+      </c>
+      <c r="B123">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>4</v>
+      </c>
+      <c r="B124">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>5</v>
+      </c>
+      <c r="B125">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>2</v>
+      </c>
+      <c r="B126">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>3</v>
+      </c>
+      <c r="B127">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>4</v>
+      </c>
+      <c r="B128">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>5</v>
+      </c>
+      <c r="B129">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>2</v>
+      </c>
+      <c r="B130">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>3</v>
+      </c>
+      <c r="B131">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>4</v>
+      </c>
+      <c r="B132">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>5</v>
+      </c>
+      <c r="B133">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>